<commit_message>
Created the Jupyter Notebook for this project. Completed a purpose section and most of a draft of the section explaining the format of the spreadsheets in the Timeline-Workbook that this application will need. Cleaned up tne included demo workbook, Timeline-Workbook, to conform to these requirements.
</commit_message>
<xml_diff>
--- a/data/Timeline-Workbook.xlsx
+++ b/data/Timeline-Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\eBooks\Games\GM Resources\Timeline Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC5102-5586-4319-872E-9E10DE0FD625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E112D09-22A1-4404-AFE5-20F3C2A51785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13515" yWindow="1665" windowWidth="14985" windowHeight="13920" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14610" yWindow="975" windowWidth="15390" windowHeight="13920" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Timelines" sheetId="1" r:id="rId1"/>
@@ -41,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="292">
-  <si>
-    <t>Race</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="289">
   <si>
     <t>Start</t>
   </si>
@@ -110,18 +107,6 @@
   </si>
   <si>
     <t>Roll</t>
-  </si>
-  <si>
-    <t>Violence</t>
-  </si>
-  <si>
-    <t>Hardship</t>
-  </si>
-  <si>
-    <t>Diplomacy</t>
-  </si>
-  <si>
-    <t>Exploration</t>
   </si>
   <si>
     <t>Peaceful trade agreement with neighboring kingdom</t>
@@ -518,10 +503,6 @@
     <t>Determine the history of these "finds" and their scope. Some could substantial, like the Trains.</t>
   </si>
   <si>
-    <t>+Trains
-+Underdark</t>
-  </si>
-  <si>
     <t>These area are unlikely  to be fully depleted, and will continue to attract denizens</t>
   </si>
   <si>
@@ -968,6 +949,16 @@
   </si>
   <si>
     <t>Depends on developing strife in the relation over decades</t>
+  </si>
+  <si>
+    <t>Regional Group</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>+Ancient Tech
++Underdark</t>
   </si>
 </sst>
 </file>
@@ -1135,14 +1126,6 @@
   <dxfs count="4">
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <gradientFill degree="90">
           <stop position="0">
             <color theme="0"/>
@@ -1213,6 +1196,14 @@
         </gradientFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1227,10 +1218,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2DDA61A-708C-8D47-A6BD-75A5EB3F5811}" name="Table1" displayName="Table1" ref="B1:C17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="3" headerRowCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2DDA61A-708C-8D47-A6BD-75A5EB3F5811}" name="Table1" displayName="Table1" ref="B1:C17" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{CBB1CD79-03A6-8145-A14E-B330F5F13907}" name="Major Period" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{B2C9A885-4647-6442-BC7A-881C60A2E857}" name="Start" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CBB1CD79-03A6-8145-A14E-B330F5F13907}" name="Major Period" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{B2C9A885-4647-6442-BC7A-881C60A2E857}" name="Start" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1536,7 +1527,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,30 +1538,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="14">
         <v>-50000</v>
@@ -1587,10 +1578,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="14">
         <v>-27000</v>
@@ -1607,10 +1598,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="14">
         <v>-25000</v>
@@ -1627,10 +1618,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="14">
         <v>0</v>
@@ -1647,10 +1638,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="14">
         <v>150</v>
@@ -1667,10 +1658,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="14">
         <v>300</v>
@@ -1687,10 +1678,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="14">
         <v>700</v>
@@ -1707,10 +1698,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="14">
         <v>-8000</v>
@@ -1727,10 +1718,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="14">
         <v>-7500</v>
@@ -1747,10 +1738,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="14">
         <v>-5500</v>
@@ -1767,10 +1758,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="14">
         <v>-8000</v>
@@ -1787,10 +1778,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="14">
         <v>-7200</v>
@@ -1807,10 +1798,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="14">
         <v>-8000</v>
@@ -1827,10 +1818,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="14">
         <v>-7500</v>
@@ -1847,10 +1838,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="14">
         <v>-2000</v>
@@ -1867,10 +1858,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="14">
         <v>-1500</v>
@@ -1910,13 +1901,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,7 +1918,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1938,7 +1929,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1949,7 +1940,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1960,7 +1951,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1971,7 +1962,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1982,7 +1973,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1993,7 +1984,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2004,7 +1995,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2015,7 +2006,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2040,13 +2031,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2057,7 +2048,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2068,7 +2059,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2079,7 +2070,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2090,7 +2081,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,7 +2092,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2112,7 +2103,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,7 +2114,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,7 +2125,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2145,7 +2136,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2156,7 +2147,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2169,10 +2160,10 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,19 +2177,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>26</v>
+        <v>287</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2206,16 +2197,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2223,16 +2214,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2240,16 +2231,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2257,16 +2248,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2274,16 +2265,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2291,16 +2282,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2308,16 +2299,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2325,16 +2316,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2342,16 +2333,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2359,16 +2350,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2376,16 +2367,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2393,16 +2384,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2419,7 +2410,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,19 +2424,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2453,16 +2444,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2470,16 +2461,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2487,16 +2478,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2504,16 +2495,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2521,16 +2512,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2538,16 +2529,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2555,16 +2546,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2572,16 +2563,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2589,16 +2580,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2606,16 +2597,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2623,16 +2614,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2640,16 +2631,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2657,16 +2648,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2674,16 +2665,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2691,16 +2682,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2708,16 +2699,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2725,16 +2716,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2748,10 +2739,10 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,19 +2756,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>24</v>
+        <v>287</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2785,16 +2776,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2802,16 +2793,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2819,16 +2810,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2836,16 +2827,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2853,16 +2844,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2870,16 +2861,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2887,16 +2878,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2904,16 +2895,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2921,16 +2912,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2938,16 +2929,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2955,16 +2946,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2972,16 +2963,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2989,16 +2980,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3006,16 +2997,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3029,10 +3020,10 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD14"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3040,25 +3031,25 @@
     <col min="1" max="1" width="5.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="36" style="12" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3066,16 +3057,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3083,16 +3074,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3100,16 +3091,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3117,16 +3108,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3134,16 +3125,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3151,16 +3142,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3168,16 +3159,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3185,16 +3176,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3202,16 +3193,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>151</v>
+        <v>288</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3219,16 +3210,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3236,16 +3227,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3271,13 +3262,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3288,7 +3279,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3299,7 +3290,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3310,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3321,7 +3312,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3332,7 +3323,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3343,7 +3334,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3354,7 +3345,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3365,7 +3356,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3376,7 +3367,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3387,7 +3378,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3412,10 +3403,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3423,7 +3414,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3431,7 +3422,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3439,7 +3430,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3447,7 +3438,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3455,7 +3446,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3481,16 +3472,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3501,10 +3492,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3515,10 +3506,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3529,10 +3520,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3543,10 +3534,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3557,10 +3548,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3571,10 +3562,10 @@
         <v>26</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3585,10 +3576,10 @@
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3599,10 +3590,10 @@
         <v>26</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3613,10 +3604,10 @@
         <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3627,10 +3618,10 @@
         <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3659,13 +3650,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3676,7 +3667,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3687,7 +3678,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3698,7 +3689,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3709,7 +3700,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3720,7 +3711,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3731,7 +3722,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3742,7 +3733,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3753,7 +3744,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3764,7 +3755,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3775,7 +3766,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3786,7 +3777,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,7 +3788,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3808,7 +3799,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3819,7 +3810,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on more descriptions of the keywords and how the application will use them. Updated the workbook to conform to this api.
</commit_message>
<xml_diff>
--- a/data/Timeline-Workbook.xlsx
+++ b/data/Timeline-Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\eBooks\Games\GM Resources\Timeline Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E112D09-22A1-4404-AFE5-20F3C2A51785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04C4ACB-4787-446D-A299-4E964ACA993A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14610" yWindow="975" windowWidth="15390" windowHeight="13920" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13410" yWindow="975" windowWidth="15390" windowHeight="13920" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Timelines" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Adventure Site" sheetId="6" r:id="rId6"/>
     <sheet name="Military" sheetId="7" r:id="rId7"/>
     <sheet name="Magic Area or School" sheetId="8" r:id="rId8"/>
-    <sheet name="Enemies" sheetId="9" r:id="rId9"/>
-    <sheet name="Status Groups" sheetId="10" r:id="rId10"/>
+    <sheet name="Enemy Options" sheetId="9" r:id="rId9"/>
+    <sheet name="Priviledged or Persecuted" sheetId="10" r:id="rId10"/>
     <sheet name="Religion Status" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="290">
   <si>
     <t>Start</t>
   </si>
@@ -959,6 +959,9 @@
   <si>
     <t>+Ancient Tech
 +Underdark</t>
+  </si>
+  <si>
+    <t>Basic Guard only</t>
   </si>
 </sst>
 </file>
@@ -2407,7 +2410,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
@@ -2739,7 +2742,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
@@ -3019,11 +3022,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B111ED2B-0572-43DB-BD97-2BACFDCEF423}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,10 +3392,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49235D1C-5B0B-49E2-9B58-4C3F23A510F3}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,41 +3414,49 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>222</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3459,7 +3470,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Verified that the first code cell loads the excel workbook, parses it correctly, and loads the correct worksheets into the right dictionaries of dataframes.
</commit_message>
<xml_diff>
--- a/data/Timeline-Workbook.xlsx
+++ b/data/Timeline-Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\eBooks\Games\GM Resources\Timeline Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04C4ACB-4787-446D-A299-4E964ACA993A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F25F338-D766-4EF9-9A7F-84A5CDF8B14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13410" yWindow="975" windowWidth="15390" windowHeight="13920" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13410" yWindow="975" windowWidth="15390" windowHeight="13920" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Timelines" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Military" sheetId="7" r:id="rId7"/>
     <sheet name="Magic Area or School" sheetId="8" r:id="rId8"/>
     <sheet name="Enemy Options" sheetId="9" r:id="rId9"/>
-    <sheet name="Priviledged or Persecuted" sheetId="10" r:id="rId10"/>
+    <sheet name="Privileged or Persecuted" sheetId="10" r:id="rId10"/>
     <sheet name="Religion Status" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="281">
   <si>
     <t>Start</t>
   </si>
@@ -774,9 +774,6 @@
     <t>Add an Air Force to the Navy</t>
   </si>
   <si>
-    <t>New Military Type</t>
-  </si>
-  <si>
     <t>Levels</t>
   </si>
   <si>
@@ -789,9 +786,6 @@
     <t>Conjuration</t>
   </si>
   <si>
-    <t>Elementalism</t>
-  </si>
-  <si>
     <t>Divination</t>
   </si>
   <si>
@@ -810,9 +804,6 @@
     <t>Transmutation</t>
   </si>
   <si>
-    <t>Summoning</t>
-  </si>
-  <si>
     <t>A necromancer and his undead army</t>
   </si>
   <si>
@@ -919,30 +910,6 @@
   </si>
   <si>
     <t>Use another method</t>
-  </si>
-  <si>
-    <t>Elven Magic System</t>
-  </si>
-  <si>
-    <t>Mind</t>
-  </si>
-  <si>
-    <t>Abnegation</t>
-  </si>
-  <si>
-    <t>Clairsentience</t>
-  </si>
-  <si>
-    <t>Gravity</t>
-  </si>
-  <si>
-    <t>Essence</t>
-  </si>
-  <si>
-    <t>Roll twice ignoring this result</t>
-  </si>
-  <si>
-    <t>Ignore this result</t>
   </si>
   <si>
     <t>Max</t>
@@ -962,6 +929,12 @@
   </si>
   <si>
     <t>Basic Guard only</t>
+  </si>
+  <si>
+    <t>This event is only a rumor.</t>
+  </si>
+  <si>
+    <t>Military Development</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1514,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>5</v>
@@ -1907,10 +1880,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1921,7 +1894,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1932,7 +1905,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1954,7 +1927,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1965,7 +1938,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1976,7 +1949,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1987,7 +1960,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1998,7 +1971,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2009,7 +1982,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2021,9 +1994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61D916A-71FC-4AD9-BCDB-8E9456D6B66C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2037,10 +2008,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2051,7 +2022,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2062,7 +2033,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2073,7 +2044,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2084,7 +2055,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2095,7 +2066,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2106,7 +2077,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2117,7 +2088,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2128,7 +2099,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2139,7 +2110,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2150,7 +2121,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2154,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>27</v>
@@ -2430,7 +2401,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>27</v>
@@ -2762,7 +2733,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>27</v>
@@ -3043,7 +3014,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>27</v>
@@ -3069,7 +3040,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3202,7 +3173,7 @@
         <v>145</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>146</v>
@@ -3268,7 +3239,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>212</v>
@@ -3337,7 +3308,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3395,7 +3366,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,10 +3377,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3417,7 +3388,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3467,10 +3438,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8DFCA4-6419-4E10-90CD-56030A1FF578}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3478,24 +3449,20 @@
     <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -3503,13 +3470,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>3</v>
       </c>
@@ -3517,13 +3481,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>7</v>
       </c>
@@ -3531,13 +3492,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>11</v>
       </c>
@@ -3545,13 +3503,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>15</v>
       </c>
@@ -3559,13 +3514,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>25</v>
       </c>
@@ -3573,13 +3525,10 @@
         <v>26</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>21</v>
       </c>
@@ -3587,13 +3536,10 @@
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>25</v>
       </c>
@@ -3601,13 +3547,10 @@
         <v>26</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>25</v>
       </c>
@@ -3615,30 +3558,10 @@
         <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <v>27</v>
-      </c>
-      <c r="B11" s="16">
-        <v>27</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D10">
-    <sortCondition ref="D2:D10"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3664,10 +3587,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3678,7 +3601,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3689,7 +3612,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3700,7 +3623,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3711,7 +3634,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3722,7 +3645,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3733,7 +3656,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3744,7 +3667,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3755,7 +3678,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3766,7 +3689,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3777,7 +3700,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3788,7 +3711,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3799,7 +3722,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3810,7 +3733,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3821,7 +3744,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected an error in two for loops that needed to loop for every group-period pairing, including the main for loop for timeline generation. Created the parsing code for the single row dataframe with new primary events. Added event_ctr to count events and number rows in the event. Updated instructions to indicate that keywords in the worksheets should be separated by newlines inserted via a spreadsheet program. Fully tested new function process_keyword which breaks up the 'Effects' column entry and finds keywors, non-keywords, and increases. Created pass versions of process_secondary_events and military_status. Created actual demo values for Base Timelines worksheet. Full successful test of appending data to df_regional_timelines dataframes.
</commit_message>
<xml_diff>
--- a/data/Timeline-Workbook.xlsx
+++ b/data/Timeline-Workbook.xlsx
@@ -5,15 +5,15 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\eBooks\Games\GM Resources\Timeline Generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\history-skeleton-generator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F25F338-D766-4EF9-9A7F-84A5CDF8B14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71147EB3-7858-46D7-8AE6-FAC850D3D8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13410" yWindow="975" windowWidth="15390" windowHeight="13920" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14640" yWindow="1845" windowWidth="15390" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Base Timelines" sheetId="1" r:id="rId1"/>
+    <sheet name="Base Timelines" sheetId="13" r:id="rId1"/>
     <sheet name="Exploration Events" sheetId="2" r:id="rId2"/>
     <sheet name="Violent Events" sheetId="3" r:id="rId3"/>
     <sheet name="Hardship Events" sheetId="4" r:id="rId4"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="281">
   <si>
     <t>Start</t>
   </si>
@@ -52,58 +52,13 @@
     <t>Period Length</t>
   </si>
   <si>
-    <t>Elves</t>
-  </si>
-  <si>
-    <t>Elves Dark</t>
-  </si>
-  <si>
     <t>Major Period</t>
   </si>
   <si>
-    <t>Pre-Desecration</t>
-  </si>
-  <si>
-    <t>Post-Desecration</t>
-  </si>
-  <si>
-    <t>Humans</t>
-  </si>
-  <si>
-    <t>Pre-Migration</t>
-  </si>
-  <si>
-    <t>Migration</t>
-  </si>
-  <si>
-    <t>Post-Migration</t>
-  </si>
-  <si>
     <t>Range</t>
   </si>
   <si>
-    <t>Humans Kingdoms</t>
-  </si>
-  <si>
-    <t>Human Baronies</t>
-  </si>
-  <si>
-    <t>Human Pirate Kingdoms</t>
-  </si>
-  <si>
-    <t>Goblin</t>
-  </si>
-  <si>
-    <t>Halflings (Goblins)</t>
-  </si>
-  <si>
     <t>Trolls</t>
-  </si>
-  <si>
-    <t>Orcs (Trolls)</t>
-  </si>
-  <si>
-    <t>Dwarves</t>
   </si>
   <si>
     <t>Roll</t>
@@ -935,6 +890,51 @@
   </si>
   <si>
     <t>Military Development</t>
+  </si>
+  <si>
+    <t>Elven Kingdom</t>
+  </si>
+  <si>
+    <t>Monarchy</t>
+  </si>
+  <si>
+    <t>High Elven Barony</t>
+  </si>
+  <si>
+    <t>Ascendency</t>
+  </si>
+  <si>
+    <t>Dwarven High Kingdom</t>
+  </si>
+  <si>
+    <t>Rise of the Emir</t>
+  </si>
+  <si>
+    <t>Dwarven Wanderers</t>
+  </si>
+  <si>
+    <t>Dispersal</t>
+  </si>
+  <si>
+    <t>Human Monarchy of Arden</t>
+  </si>
+  <si>
+    <t>Tiefling</t>
+  </si>
+  <si>
+    <t>Rise of Warlocks</t>
+  </si>
+  <si>
+    <t>Halfing Protectorate</t>
+  </si>
+  <si>
+    <t>Feet of Clay</t>
+  </si>
+  <si>
+    <t>Orc Northern Hegemony</t>
+  </si>
+  <si>
+    <t>Fires of Doom</t>
   </si>
 </sst>
 </file>
@@ -958,22 +958,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <gradientFill degree="90">
-        <stop position="0">
-          <color theme="0"/>
-        </stop>
-        <stop position="1">
-          <color theme="0"/>
-        </stop>
-      </gradientFill>
     </fill>
   </fills>
   <borders count="4">
@@ -1062,7 +1052,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1084,103 +1073,29 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1191,16 +1106,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2DDA61A-708C-8D47-A6BD-75A5EB3F5811}" name="Table1" displayName="Table1" ref="B1:C17" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Normal">
-  <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{CBB1CD79-03A6-8145-A14E-B330F5F13907}" name="Major Period" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{B2C9A885-4647-6442-BC7A-881C60A2E857}" name="Start" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1499,364 +1404,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A697FEA4-79A6-E94A-BFEE-59560E40E063}">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31629C1-FE9F-4FEF-ADA6-2856507A55CA}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="24"/>
+    <col min="5" max="5" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>5</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>12</v>
+      <c r="F1" s="21" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="14">
-        <v>-50000</v>
-      </c>
-      <c r="D2" s="14">
-        <v>200</v>
-      </c>
-      <c r="E2" s="14">
-        <v>150</v>
-      </c>
-      <c r="F2" s="14">
+      <c r="A2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="26">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="26">
+        <v>2000</v>
+      </c>
+      <c r="E2" s="25">
+        <v>100</v>
+      </c>
+      <c r="F2" s="25">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="14">
-        <v>-27000</v>
-      </c>
-      <c r="D3" s="14">
-        <v>-25000</v>
-      </c>
-      <c r="E3" s="14">
-        <v>150</v>
-      </c>
-      <c r="F3" s="14">
+      <c r="A3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="26">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="26">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="25">
+        <v>100</v>
+      </c>
+      <c r="F3" s="25">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="14">
-        <v>-25000</v>
-      </c>
-      <c r="D4" s="14">
+      <c r="A4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1550</v>
+      </c>
+      <c r="D4" s="26">
         <v>2000</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="25">
+        <v>75</v>
+      </c>
+      <c r="F4" s="25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="26">
+        <v>1200</v>
+      </c>
+      <c r="D5" s="26">
+        <v>1550</v>
+      </c>
+      <c r="E5" s="25">
+        <v>75</v>
+      </c>
+      <c r="F5" s="25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="26">
         <v>1000</v>
       </c>
-      <c r="F4" s="14">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>150</v>
-      </c>
-      <c r="E5" s="14">
-        <v>50</v>
-      </c>
-      <c r="F5" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="14">
-        <v>150</v>
-      </c>
-      <c r="D6" s="14">
+      <c r="D6" s="26">
+        <v>1800</v>
+      </c>
+      <c r="E6" s="25">
+        <v>65</v>
+      </c>
+      <c r="F6" s="25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" s="26">
+        <v>1550</v>
+      </c>
+      <c r="D7" s="26">
         <v>2000</v>
       </c>
-      <c r="E6" s="14">
-        <v>100</v>
-      </c>
-      <c r="F6" s="14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="14">
-        <v>300</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="E7" s="25">
+        <v>75</v>
+      </c>
+      <c r="F7" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1550</v>
+      </c>
+      <c r="D8" s="26">
         <v>2000</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E8" s="25">
         <v>65</v>
       </c>
-      <c r="F7" s="14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="14">
-        <v>700</v>
-      </c>
-      <c r="D8" s="14">
+      <c r="F8" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="26">
+        <v>1400</v>
+      </c>
+      <c r="D9" s="26">
         <v>2000</v>
       </c>
-      <c r="E8" s="14">
-        <v>60</v>
-      </c>
-      <c r="F8" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="14">
-        <v>-8000</v>
-      </c>
-      <c r="D9" s="14">
-        <v>-7500</v>
-      </c>
-      <c r="E9" s="14">
-        <v>50</v>
-      </c>
-      <c r="F9" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="14">
-        <v>-7500</v>
-      </c>
-      <c r="D10" s="14">
-        <v>2000</v>
-      </c>
-      <c r="E10" s="14">
-        <v>100</v>
-      </c>
-      <c r="F10" s="14">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="14">
-        <v>-5500</v>
-      </c>
-      <c r="D11" s="14">
-        <v>2000</v>
-      </c>
-      <c r="E11" s="14">
-        <v>50</v>
-      </c>
-      <c r="F11" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="14">
-        <v>-8000</v>
-      </c>
-      <c r="D12" s="14">
-        <v>-7200</v>
-      </c>
-      <c r="E12" s="14">
-        <v>100</v>
-      </c>
-      <c r="F12" s="14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="14">
-        <v>-7200</v>
-      </c>
-      <c r="D13" s="14">
-        <v>2000</v>
-      </c>
-      <c r="E13" s="14">
-        <v>100</v>
-      </c>
-      <c r="F13" s="14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="14">
-        <v>-8000</v>
-      </c>
-      <c r="D14" s="14">
-        <v>-7500</v>
-      </c>
-      <c r="E14" s="14">
-        <v>70</v>
-      </c>
-      <c r="F14" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="14">
-        <v>-7500</v>
-      </c>
-      <c r="D15" s="14">
-        <v>2000</v>
-      </c>
-      <c r="E15" s="14">
-        <v>70</v>
-      </c>
-      <c r="F15" s="14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="14">
-        <v>-2000</v>
-      </c>
-      <c r="D16" s="14">
-        <v>-1500</v>
-      </c>
-      <c r="E16" s="14">
-        <v>70</v>
-      </c>
-      <c r="F16" s="14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="14">
-        <v>-1500</v>
-      </c>
-      <c r="D17" s="14">
-        <v>2000</v>
-      </c>
-      <c r="E17" s="14">
-        <v>70</v>
-      </c>
-      <c r="F17" s="14">
-        <v>30</v>
+      <c r="E9" s="25">
+        <v>125</v>
+      </c>
+      <c r="F9" s="25">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -1876,113 +1622,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
         <v>21</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
-        <v>21</v>
-      </c>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>23</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>24</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>25</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>26</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>27</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>28</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>30</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -1998,130 +1744,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>15</v>
+      </c>
+      <c r="B6" s="15">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15">
+        <v>20</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <v>21</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>3</v>
-      </c>
-      <c r="B3" s="16">
-        <v>6</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>7</v>
-      </c>
-      <c r="B4" s="16">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>11</v>
-      </c>
-      <c r="B5" s="16">
-        <v>14</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>15</v>
-      </c>
-      <c r="B6" s="16">
-        <v>18</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>19</v>
-      </c>
-      <c r="B7" s="16">
-        <v>20</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>21</v>
-      </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>23</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>24</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>25</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>27</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2151,19 +1897,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2171,16 +1917,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2188,16 +1934,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2205,16 +1951,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2222,16 +1968,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2239,16 +1985,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2256,16 +2002,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2273,16 +2019,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2290,16 +2036,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2307,16 +2053,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2324,16 +2070,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2341,16 +2087,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2358,16 +2104,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2398,19 +2144,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2418,16 +2164,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2435,16 +2181,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2452,16 +2198,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2469,16 +2215,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2486,16 +2232,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2503,16 +2249,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2520,16 +2266,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2537,16 +2283,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2554,16 +2300,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2571,16 +2317,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2588,16 +2334,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2605,16 +2351,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2622,16 +2368,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2639,16 +2385,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2656,16 +2402,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2673,16 +2419,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2690,16 +2436,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2730,19 +2476,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2750,16 +2496,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2767,16 +2513,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2784,16 +2530,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2801,16 +2547,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2818,16 +2564,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2835,16 +2581,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2852,16 +2598,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2869,16 +2615,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2886,16 +2632,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2903,16 +2649,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2920,16 +2666,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2937,16 +2683,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2954,16 +2700,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2971,16 +2717,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3011,19 +2757,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3031,16 +2777,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3048,16 +2794,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3065,16 +2811,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3082,16 +2828,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3099,16 +2845,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3116,16 +2862,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3133,16 +2879,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3150,16 +2896,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3167,16 +2913,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3184,16 +2930,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3201,16 +2947,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3235,124 +2981,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>15</v>
+      </c>
+      <c r="B6" s="15">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <v>21</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>3</v>
-      </c>
-      <c r="B3" s="16">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>7</v>
-      </c>
-      <c r="B4" s="16">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>11</v>
-      </c>
-      <c r="B5" s="16">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>15</v>
-      </c>
-      <c r="B6" s="16">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>19</v>
-      </c>
-      <c r="B7" s="16">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>21</v>
-      </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>23</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>25</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>27</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3365,7 +3111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49235D1C-5B0B-49E2-9B58-4C3F23A510F3}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3377,10 +3123,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3388,7 +3134,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3396,7 +3142,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3404,7 +3150,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3412,7 +3158,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3420,7 +3166,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3428,7 +3174,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3452,113 +3198,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>15</v>
+      </c>
+      <c r="B6" s="15">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>25</v>
+      </c>
+      <c r="B7" s="15">
+        <v>26</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <v>21</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>3</v>
-      </c>
-      <c r="B3" s="16">
-        <v>6</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>7</v>
-      </c>
-      <c r="B4" s="16">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>11</v>
-      </c>
-      <c r="B5" s="16">
-        <v>14</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>15</v>
-      </c>
-      <c r="B6" s="16">
-        <v>18</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="B8" s="15">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
         <v>25</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B9" s="15">
         <v>26</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>21</v>
-      </c>
-      <c r="B8" s="16">
-        <v>22</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="C9" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
         <v>25</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B10" s="15">
         <v>26</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
-        <v>25</v>
-      </c>
-      <c r="B10" s="16">
-        <v>26</v>
-      </c>
       <c r="C10" s="9" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3583,168 +3329,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>3</v>
+      </c>
+      <c r="B3" s="18">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>9</v>
+      </c>
+      <c r="B6" s="18">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>11</v>
+      </c>
+      <c r="B7" s="18">
+        <v>12</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>13</v>
+      </c>
+      <c r="B8" s="18">
+        <v>14</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>15</v>
+      </c>
+      <c r="B9" s="18">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>17</v>
+      </c>
+      <c r="B10" s="18">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>19</v>
+      </c>
+      <c r="B11" s="18">
+        <v>20</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>21</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
-        <v>1</v>
-      </c>
-      <c r="B2" s="19">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
-        <v>3</v>
-      </c>
-      <c r="B3" s="19">
-        <v>4</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
-        <v>5</v>
-      </c>
-      <c r="B4" s="19">
-        <v>6</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
-        <v>7</v>
-      </c>
-      <c r="B5" s="19">
-        <v>8</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
-        <v>9</v>
-      </c>
-      <c r="B6" s="19">
-        <v>10</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
-        <v>11</v>
-      </c>
-      <c r="B7" s="19">
-        <v>12</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>13</v>
-      </c>
-      <c r="B8" s="19">
-        <v>14</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>15</v>
-      </c>
-      <c r="B9" s="19">
-        <v>16</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
-        <v>17</v>
-      </c>
-      <c r="B10" s="19">
-        <v>18</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
-        <v>19</v>
-      </c>
-      <c r="B11" s="19">
-        <v>20</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>21</v>
-      </c>
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <v>24</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <v>25</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <v>25</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="17">
         <v>26</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>26</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="A15" s="14">
         <v>27</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>27</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added constants MILITARY_COLUMNS, PRIMARY_EVENT_COLUMNS and SECONDARY_EVENTS COLUMNS to help handle validation of primary events and secondary events worksheets. Discovered a typo with persecuted in the KEYWORDS and fixed that in the code. Added tests for integer values in the Roll columns of primary events workbooks  and Roll and Max columns of secondary events workbooks. Added duplicate entry checks for Military worksheets and all primary events sheets. Testing also prevents Roll and Max columns in secondary events worksheets from overlapping or duplicating results. These have been fully tested to ensure that they prevent bad workbooks from being processed. Timeline-Workbook has the broken changes corrected for the demo.
</commit_message>
<xml_diff>
--- a/data/Timeline-Workbook.xlsx
+++ b/data/Timeline-Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\history-skeleton-generator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71147EB3-7858-46D7-8AE6-FAC850D3D8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5063901C-5500-42B5-848D-0A8D1F98CE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14640" yWindow="1845" windowWidth="15390" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7620" yWindow="1515" windowWidth="21180" windowHeight="13920" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Timelines" sheetId="13" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="282">
   <si>
     <t>Start</t>
   </si>
@@ -935,6 +935,9 @@
   </si>
   <si>
     <t>Fires of Doom</t>
+  </si>
+  <si>
+    <t>Universal</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31629C1-FE9F-4FEF-ADA6-2856507A55CA}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1611,7 +1614,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,6 +1735,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
+    <sortCondition ref="A2:A10"/>
+    <sortCondition ref="B2:B10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1740,7 +1747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61D916A-71FC-4AD9-BCDB-8E9456D6B66C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3184,10 +3191,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8DFCA4-6419-4E10-90CD-56030A1FF578}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,7 +3231,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>215</v>
@@ -3232,10 +3239,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>216</v>
@@ -3243,10 +3250,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="15">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>217</v>
@@ -3254,10 +3261,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B6" s="15">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>218</v>
@@ -3265,10 +3272,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B7" s="15">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>219</v>
@@ -3276,10 +3283,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B8" s="15">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>220</v>
@@ -3287,10 +3294,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B9" s="15">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>221</v>
@@ -3298,12 +3305,23 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B10" s="15">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>18</v>
+      </c>
+      <c r="B11" s="15">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>264</v>
       </c>
     </row>

</xml_diff>